<commit_message>
2024.10.08 백엔드 API URL을 REST 방식으로 정리
</commit_message>
<xml_diff>
--- a/자료/Backend/11.API 정리.xlsx
+++ b/자료/Backend/11.API 정리.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild="10.105.228.52576"/>
+  <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild="9.104.180.50664"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="510" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="500" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="기능 정리" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
   <si>
     <t>기능 정리</t>
   </si>
@@ -1139,6 +1139,27 @@
   </si>
   <si>
     <t>로그인 체크 &amp; 권한 체크</t>
+  </si>
+  <si>
+    <t>/api/user</t>
+  </si>
+  <si>
+    <t>/api/user/ㅣㅐ햐ㅜ</t>
+  </si>
+  <si>
+    <t>/api/memo</t>
+  </si>
+  <si>
+    <t>/api/memos/memo</t>
+  </si>
+  <si>
+    <t>/api/memos/memo/image</t>
+  </si>
+  <si>
+    <t>/api/memo/share</t>
+  </si>
+  <si>
+    <t>/api/memo/setting</t>
   </si>
 </sst>
 </file>
@@ -1885,7 +1906,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2101,6 +2122,12 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2422,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView topLeftCell="A31" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -2578,7 +2605,7 @@
         <v>173</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H6" s="59" t="s">
         <v>188</v>
@@ -2606,7 +2633,7 @@
         <v>172</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>170</v>
+        <v>263</v>
       </c>
       <c r="H7" s="59" t="s">
         <v>189</v>
@@ -2826,7 +2853,7 @@
         <v>193</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
       <c r="H17" s="59" t="s">
         <v>195</v>
@@ -2852,7 +2879,7 @@
         <v>193</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
       <c r="H18" s="59" t="s">
         <v>186</v>
@@ -2878,7 +2905,7 @@
         <v>193</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
       <c r="H19" s="59" t="s">
         <v>196</v>
@@ -2904,7 +2931,7 @@
         <v>193</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
       <c r="H20" s="59" t="s">
         <v>197</v>
@@ -2934,7 +2961,7 @@
         <v>172</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>199</v>
+        <v>265</v>
       </c>
       <c r="H21" s="59" t="s">
         <v>200</v>
@@ -2954,21 +2981,23 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>202</v>
+        <v>235</v>
+      </c>
+      <c r="F22" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="G22" s="59" t="s">
+        <v>265</v>
       </c>
       <c r="H22" s="59" t="s">
-        <v>200</v>
+        <v>237</v>
       </c>
       <c r="I22" s="59" t="s">
-        <v>205</v>
-      </c>
-      <c r="J22" s="3"/>
+        <v>206</v>
+      </c>
+      <c r="J22" s="59" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="66.000000">
       <c r="A23" s="52"/>
@@ -2984,7 +3013,7 @@
         <v>193</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>208</v>
+        <v>265</v>
       </c>
       <c r="H23" s="59" t="s">
         <v>228</v>
@@ -3008,7 +3037,7 @@
         <v>229</v>
       </c>
       <c r="G24" s="59" t="s">
-        <v>230</v>
+        <v>265</v>
       </c>
       <c r="H24" s="59" t="s">
         <v>231</v>
@@ -3042,31 +3071,29 @@
       </c>
       <c r="J25" s="59"/>
     </row>
-    <row r="26" spans="1:10" ht="33.000000">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+    <row r="26" spans="1:10" s="72" customFormat="1" ht="33.000000">
+      <c r="A26" s="51"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="3" t="s">
         <v>166</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F26" s="59" t="s">
-        <v>173</v>
-      </c>
-      <c r="G26" s="59" t="s">
-        <v>236</v>
+        <v>201</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="H26" s="59" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="I26" s="59" t="s">
-        <v>206</v>
-      </c>
-      <c r="J26" s="59" t="s">
-        <v>238</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="J26" s="59"/>
     </row>
     <row r="27" spans="1:10" ht="33.000000">
       <c r="A27" s="51"/>
@@ -3084,7 +3111,7 @@
         <v>172</v>
       </c>
       <c r="G27" s="59" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="H27" s="59" t="s">
         <v>243</v>
@@ -3110,7 +3137,7 @@
         <v>229</v>
       </c>
       <c r="G28" s="59" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="H28" s="59" t="s">
         <v>243</v>
@@ -3136,7 +3163,7 @@
         <v>173</v>
       </c>
       <c r="G29" s="59" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="H29" s="59" t="s">
         <v>246</v>
@@ -3162,7 +3189,7 @@
         <v>193</v>
       </c>
       <c r="G30" s="59" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="H30" s="59" t="s">
         <v>251</v>
@@ -3188,7 +3215,7 @@
         <v>193</v>
       </c>
       <c r="G31" s="59" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="H31" s="59" t="s">
         <v>252</v>
@@ -3214,7 +3241,7 @@
         <v>193</v>
       </c>
       <c r="G32" s="59" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="H32" s="59" t="s">
         <v>254</v>
@@ -3240,7 +3267,7 @@
         <v>193</v>
       </c>
       <c r="G33" s="59" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="H33" s="59" t="s">
         <v>255</v>
@@ -4347,6 +4374,18 @@
       <c r="H108" s="59"/>
       <c r="I108" s="59"/>
       <c r="J108" s="59"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="0"/>
+      <c r="B109" s="0"/>
+      <c r="C109" s="0"/>
+      <c r="D109" s="0"/>
+      <c r="E109" s="0"/>
+      <c r="F109" s="0"/>
+      <c r="G109" s="0"/>
+      <c r="H109" s="57"/>
+      <c r="I109" s="57"/>
+      <c r="J109" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="31">

</xml_diff>

<commit_message>
2024-10-07 Memo Follow API 구현중
</commit_message>
<xml_diff>
--- a/자료/Backend/11.API 정리.xlsx
+++ b/자료/Backend/11.API 정리.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="278">
   <si>
     <t>기능 정리</t>
   </si>
@@ -1160,6 +1160,30 @@
   </si>
   <si>
     <t>/api/memo/setting</t>
+  </si>
+  <si>
+    <t>/api/memo/follow</t>
+  </si>
+  <si>
+    <t>/api</t>
+  </si>
+  <si>
+    <t>/api/memo/follow/memo</t>
+  </si>
+  <si>
+    <t>나중에 필요하면 추가하자</t>
+  </si>
+  <si>
+    <t>/api/memo/follow/list</t>
+  </si>
+  <si>
+    <t>팔로잉 메모 리스트 조회</t>
+  </si>
+  <si>
+    <t>/api/memo/follow/requset</t>
+  </si>
+  <si>
+    <t>/api/memo/follow/req</t>
   </si>
 </sst>
 </file>
@@ -1340,7 +1364,7 @@
       <color rgb="FFCE9178"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1554,8 +1578,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.150000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1756,6 +1792,14 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1906,7 +1950,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2128,6 +2172,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2450,7 +2509,7 @@
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView topLeftCell="A31" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -2458,7 +2517,7 @@
     <col min="2" max="2" width="22.25499916" customWidth="1" outlineLevel="0"/>
     <col min="5" max="5" width="47.63000107" customWidth="1" outlineLevel="0"/>
     <col min="6" max="6" width="20.00499916" customWidth="1" outlineLevel="0"/>
-    <col min="7" max="7" width="22.12999916" customWidth="1" outlineLevel="0"/>
+    <col min="7" max="7" width="24.12999916" customWidth="1" outlineLevel="0"/>
     <col min="8" max="8" style="57" width="20.75499916" customWidth="1" outlineLevel="0"/>
     <col min="9" max="9" style="57" width="11.88000011" customWidth="1" outlineLevel="0"/>
     <col min="10" max="10" width="36.25500107" customWidth="1" outlineLevel="0"/>
@@ -3315,8 +3374,12 @@
       <c r="E35" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
+      <c r="F35" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="59" t="s">
+        <v>270</v>
+      </c>
       <c r="H35" s="59"/>
       <c r="I35" s="59"/>
       <c r="J35" s="59"/>
@@ -3324,16 +3387,26 @@
     <row r="36" spans="1:10">
       <c r="A36" s="52"/>
       <c r="B36" s="52"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4" t="s">
+      <c r="C36" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
+      <c r="F36" s="77" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36" s="77" t="s">
+        <v>270</v>
+      </c>
+      <c r="H36" s="77"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="77" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="3"/>
@@ -3343,8 +3416,12 @@
       <c r="E37" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
+      <c r="F37" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="G37" s="59" t="s">
+        <v>270</v>
+      </c>
       <c r="H37" s="59"/>
       <c r="I37" s="59"/>
       <c r="J37" s="59"/>
@@ -3357,19 +3434,27 @@
       <c r="E38" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
+      <c r="F38" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="G38" s="59" t="s">
+        <v>270</v>
+      </c>
       <c r="H38" s="59"/>
       <c r="I38" s="59"/>
       <c r="J38" s="59"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="52"/>
-      <c r="B39" s="52"/>
+      <c r="A39" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F39" s="59"/>
       <c r="G39" s="59"/>
@@ -3378,16 +3463,12 @@
       <c r="J39" s="59"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="51" t="s">
-        <v>27</v>
-      </c>
+      <c r="A40" s="13"/>
+      <c r="B40" s="52"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F40" s="59"/>
       <c r="G40" s="59"/>
@@ -3401,7 +3482,7 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F41" s="59"/>
       <c r="G41" s="59"/>
@@ -3415,7 +3496,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F42" s="59"/>
       <c r="G42" s="59"/>
@@ -3424,12 +3505,11 @@
       <c r="J42" s="59"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="13"/>
-      <c r="B43" s="52"/>
+      <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="4" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="F43" s="59"/>
       <c r="G43" s="59"/>
@@ -3438,11 +3518,12 @@
       <c r="J43" s="59"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="B44" s="3"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F44" s="59"/>
       <c r="G44" s="59"/>
@@ -3452,11 +3533,13 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="13"/>
-      <c r="B45" s="52"/>
+      <c r="B45" s="51" t="s">
+        <v>33</v>
+      </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="4" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="F45" s="59"/>
       <c r="G45" s="59"/>
@@ -3466,13 +3549,11 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="13"/>
-      <c r="B46" s="51" t="s">
-        <v>33</v>
-      </c>
+      <c r="B46" s="52"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F46" s="59"/>
       <c r="G46" s="59"/>
@@ -3482,11 +3563,11 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="13"/>
-      <c r="B47" s="52"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F47" s="59"/>
       <c r="G47" s="59"/>
@@ -3500,7 +3581,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F48" s="59"/>
       <c r="G48" s="59"/>
@@ -3514,7 +3595,7 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F49" s="59"/>
       <c r="G49" s="59"/>
@@ -3528,7 +3609,7 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F50" s="59"/>
       <c r="G50" s="59"/>
@@ -3538,11 +3619,11 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="13"/>
-      <c r="B51" s="51"/>
+      <c r="B51" s="52"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F51" s="59"/>
       <c r="G51" s="59"/>
@@ -3552,11 +3633,13 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="13"/>
-      <c r="B52" s="52"/>
+      <c r="B52" s="51" t="s">
+        <v>40</v>
+      </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F52" s="59"/>
       <c r="G52" s="59"/>
@@ -3566,13 +3649,11 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="13"/>
-      <c r="B53" s="51" t="s">
-        <v>40</v>
-      </c>
+      <c r="B53" s="52"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F53" s="59"/>
       <c r="G53" s="59"/>
@@ -3586,7 +3667,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="4" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="F54" s="59"/>
       <c r="G54" s="59"/>
@@ -3595,12 +3676,11 @@
       <c r="J54" s="59"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="13"/>
-      <c r="B55" s="52"/>
+      <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="4" t="s">
-        <v>141</v>
+        <v>60</v>
       </c>
       <c r="F55" s="59"/>
       <c r="G55" s="59"/>
@@ -3609,11 +3689,12 @@
       <c r="J55" s="59"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="B56" s="3"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="52"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F56" s="59"/>
       <c r="G56" s="59"/>
@@ -3622,12 +3703,16 @@
       <c r="J56" s="59"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="14"/>
-      <c r="B57" s="52"/>
+      <c r="A57" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F57" s="59"/>
       <c r="G57" s="59"/>
@@ -3636,16 +3721,12 @@
       <c r="J57" s="59"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="51" t="s">
-        <v>27</v>
-      </c>
+      <c r="A58" s="13"/>
+      <c r="B58" s="52"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F58" s="59"/>
       <c r="G58" s="59"/>
@@ -3659,7 +3740,7 @@
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F59" s="59"/>
       <c r="G59" s="59"/>
@@ -3673,7 +3754,7 @@
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F60" s="59"/>
       <c r="G60" s="59"/>
@@ -3682,12 +3763,11 @@
       <c r="J60" s="59"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="13"/>
-      <c r="B61" s="52"/>
+      <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="4" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="F61" s="59"/>
       <c r="G61" s="59"/>
@@ -3700,7 +3780,7 @@
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F62" s="59"/>
       <c r="G62" s="59"/>
@@ -3709,11 +3789,12 @@
       <c r="J62" s="59"/>
     </row>
     <row r="63" spans="1:10">
-      <c r="B63" s="3"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="52"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F63" s="59"/>
       <c r="G63" s="59"/>
@@ -3723,11 +3804,13 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="13"/>
-      <c r="B64" s="52"/>
+      <c r="B64" s="51" t="s">
+        <v>33</v>
+      </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="4" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="F64" s="59"/>
       <c r="G64" s="59"/>
@@ -3737,13 +3820,11 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="13"/>
-      <c r="B65" s="51" t="s">
-        <v>33</v>
-      </c>
+      <c r="B65" s="52"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F65" s="59"/>
       <c r="G65" s="59"/>
@@ -3757,7 +3838,7 @@
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F66" s="59"/>
       <c r="G66" s="59"/>
@@ -3771,7 +3852,7 @@
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F67" s="59"/>
       <c r="G67" s="59"/>
@@ -3785,7 +3866,7 @@
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F68" s="59"/>
       <c r="G68" s="59"/>
@@ -3799,7 +3880,7 @@
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F69" s="59"/>
       <c r="G69" s="59"/>
@@ -3809,11 +3890,11 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="13"/>
-      <c r="B70" s="52"/>
+      <c r="B70" s="51"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F70" s="59"/>
       <c r="G70" s="59"/>
@@ -3826,8 +3907,8 @@
       <c r="B71" s="51"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="4" t="s">
-        <v>73</v>
+      <c r="E71" s="46" t="s">
+        <v>74</v>
       </c>
       <c r="F71" s="59"/>
       <c r="G71" s="59"/>
@@ -3841,7 +3922,7 @@
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F72" s="59"/>
       <c r="G72" s="59"/>
@@ -3851,11 +3932,13 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="13"/>
-      <c r="B73" s="51"/>
+      <c r="B73" s="51" t="s">
+        <v>40</v>
+      </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
-      <c r="E73" s="46" t="s">
-        <v>75</v>
+      <c r="E73" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="F73" s="59"/>
       <c r="G73" s="59"/>
@@ -3865,13 +3948,11 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="13"/>
-      <c r="B74" s="51" t="s">
-        <v>40</v>
-      </c>
+      <c r="B74" s="52"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F74" s="59"/>
       <c r="G74" s="59"/>
@@ -3880,12 +3961,11 @@
       <c r="J74" s="59"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="13"/>
-      <c r="B75" s="52"/>
+      <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="4" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="F75" s="59"/>
       <c r="G75" s="59"/>
@@ -3894,11 +3974,12 @@
       <c r="J75" s="59"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="B76" s="3"/>
+      <c r="A76" s="13"/>
+      <c r="B76" s="52"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="4" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="F76" s="59"/>
       <c r="G76" s="59"/>
@@ -3907,12 +3988,12 @@
       <c r="J76" s="59"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="13"/>
+      <c r="A77" s="14"/>
       <c r="B77" s="52"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F77" s="59"/>
       <c r="G77" s="59"/>
@@ -3921,12 +4002,16 @@
       <c r="J77" s="59"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="14"/>
-      <c r="B78" s="52"/>
+      <c r="A78" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F78" s="59"/>
       <c r="G78" s="59"/>
@@ -3935,16 +4020,12 @@
       <c r="J78" s="59"/>
     </row>
     <row r="79" spans="1:10">
-      <c r="A79" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B79" s="51" t="s">
-        <v>27</v>
-      </c>
+      <c r="A79" s="13"/>
+      <c r="B79" s="52"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F79" s="59"/>
       <c r="G79" s="59"/>
@@ -3958,7 +4039,7 @@
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F80" s="59"/>
       <c r="G80" s="59"/>
@@ -3972,7 +4053,7 @@
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="4" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="F81" s="59"/>
       <c r="G81" s="59"/>
@@ -3986,7 +4067,7 @@
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F82" s="59"/>
       <c r="G82" s="59"/>
@@ -3995,12 +4076,13 @@
       <c r="J82" s="59"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="13"/>
-      <c r="B83" s="52"/>
+      <c r="B83" s="52" t="s">
+        <v>33</v>
+      </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F83" s="59"/>
       <c r="G83" s="59"/>
@@ -4009,13 +4091,11 @@
       <c r="J83" s="59"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="B84" s="52" t="s">
-        <v>33</v>
-      </c>
+      <c r="B84" s="52"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F84" s="59"/>
       <c r="G84" s="59"/>
@@ -4024,11 +4104,14 @@
       <c r="J84" s="59"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="B85" s="52"/>
+      <c r="A85" s="13"/>
+      <c r="B85" s="51" t="s">
+        <v>40</v>
+      </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="4" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="F85" s="59"/>
       <c r="G85" s="59"/>
@@ -4038,13 +4121,11 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="13"/>
-      <c r="B86" s="51" t="s">
-        <v>40</v>
-      </c>
+      <c r="B86" s="52"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F86" s="59"/>
       <c r="G86" s="59"/>
@@ -4053,12 +4134,11 @@
       <c r="J86" s="59"/>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="13"/>
-      <c r="B87" s="52"/>
+      <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="4" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="F87" s="59"/>
       <c r="G87" s="59"/>
@@ -4067,11 +4147,12 @@
       <c r="J87" s="59"/>
     </row>
     <row r="88" spans="1:10">
-      <c r="B88" s="3"/>
+      <c r="A88" s="13"/>
+      <c r="B88" s="52"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="4" t="s">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="F88" s="59"/>
       <c r="G88" s="59"/>
@@ -4085,7 +4166,7 @@
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F89" s="59"/>
       <c r="G89" s="59"/>
@@ -4094,12 +4175,12 @@
       <c r="J89" s="59"/>
     </row>
     <row r="90" spans="1:10">
-      <c r="A90" s="13"/>
+      <c r="A90" s="14"/>
       <c r="B90" s="52"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F90" s="59"/>
       <c r="G90" s="59"/>
@@ -4108,12 +4189,16 @@
       <c r="J90" s="59"/>
     </row>
     <row r="91" spans="1:10">
-      <c r="A91" s="14"/>
-      <c r="B91" s="52"/>
+      <c r="A91" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F91" s="59"/>
       <c r="G91" s="59"/>
@@ -4122,16 +4207,12 @@
       <c r="J91" s="59"/>
     </row>
     <row r="92" spans="1:10">
-      <c r="A92" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B92" s="51" t="s">
-        <v>27</v>
-      </c>
+      <c r="A92" s="13"/>
+      <c r="B92" s="51"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="4" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="F92" s="59"/>
       <c r="G92" s="59"/>
@@ -4145,7 +4226,7 @@
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="4" t="s">
-        <v>160</v>
+        <v>99</v>
       </c>
       <c r="F93" s="59"/>
       <c r="G93" s="59"/>
@@ -4159,7 +4240,7 @@
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="4" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="F94" s="59"/>
       <c r="G94" s="59"/>
@@ -4173,7 +4254,7 @@
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F95" s="59"/>
       <c r="G95" s="59"/>
@@ -4183,11 +4264,13 @@
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="13"/>
-      <c r="B96" s="51"/>
+      <c r="B96" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="4" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F96" s="59"/>
       <c r="G96" s="59"/>
@@ -4196,14 +4279,12 @@
       <c r="J96" s="59"/>
     </row>
     <row r="97" spans="1:10">
-      <c r="A97" s="13"/>
-      <c r="B97" s="51" t="s">
-        <v>102</v>
-      </c>
+      <c r="A97" s="14"/>
+      <c r="B97" s="52"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F97" s="59"/>
       <c r="G97" s="59"/>
@@ -4212,12 +4293,16 @@
       <c r="J97" s="59"/>
     </row>
     <row r="98" spans="1:10">
-      <c r="A98" s="14"/>
-      <c r="B98" s="52"/>
+      <c r="A98" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="4" t="s">
-        <v>159</v>
+        <v>92</v>
       </c>
       <c r="F98" s="59"/>
       <c r="G98" s="59"/>
@@ -4226,16 +4311,12 @@
       <c r="J98" s="59"/>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B99" s="51" t="s">
-        <v>27</v>
-      </c>
+      <c r="A99" s="40"/>
+      <c r="B99" s="52"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F99" s="59"/>
       <c r="G99" s="59"/>
@@ -4249,7 +4330,7 @@
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F100" s="59"/>
       <c r="G100" s="59"/>
@@ -4263,7 +4344,7 @@
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F101" s="59"/>
       <c r="G101" s="59"/>
@@ -4272,12 +4353,14 @@
       <c r="J101" s="59"/>
     </row>
     <row r="102" spans="1:10">
-      <c r="A102" s="40"/>
-      <c r="B102" s="52"/>
+      <c r="A102" s="29"/>
+      <c r="B102" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
-      <c r="E102" s="4" t="s">
-        <v>95</v>
+      <c r="E102" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="F102" s="59"/>
       <c r="G102" s="59"/>
@@ -4287,13 +4370,11 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="29"/>
-      <c r="B103" s="51" t="s">
-        <v>102</v>
-      </c>
+      <c r="B103" s="52"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F103" s="59"/>
       <c r="G103" s="59"/>
@@ -4302,12 +4383,16 @@
       <c r="J103" s="59"/>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="29"/>
-      <c r="B104" s="52"/>
+      <c r="A104" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B104" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
-      <c r="E104" s="3" t="s">
-        <v>118</v>
+      <c r="E104" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="F104" s="59"/>
       <c r="G104" s="59"/>
@@ -4316,16 +4401,12 @@
       <c r="J104" s="59"/>
     </row>
     <row r="105" spans="1:10">
-      <c r="A105" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="B105" s="51" t="s">
-        <v>27</v>
-      </c>
+      <c r="A105" s="40"/>
+      <c r="B105" s="52"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F105" s="59"/>
       <c r="G105" s="59"/>
@@ -4339,7 +4420,7 @@
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F106" s="59"/>
       <c r="G106" s="59"/>
@@ -4353,7 +4434,7 @@
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F107" s="59"/>
       <c r="G107" s="59"/>
@@ -4362,18 +4443,16 @@
       <c r="J107" s="59"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="40"/>
-      <c r="B108" s="52"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F108" s="59"/>
-      <c r="G108" s="59"/>
-      <c r="H108" s="59"/>
-      <c r="I108" s="59"/>
-      <c r="J108" s="59"/>
+      <c r="A108" s="0"/>
+      <c r="B108" s="0"/>
+      <c r="C108" s="0"/>
+      <c r="D108" s="0"/>
+      <c r="E108" s="0"/>
+      <c r="F108" s="0"/>
+      <c r="G108" s="0"/>
+      <c r="H108" s="57"/>
+      <c r="I108" s="57"/>
+      <c r="J108" s="0"/>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="0"/>
@@ -4396,30 +4475,30 @@
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A21:A39"/>
+    <mergeCell ref="A21:A38"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="B27:B34"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="A40:A57"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="A58:A78"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B65:B73"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="A79:A91"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="A92:A98"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A99:A104"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A39:A56"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="A57:A77"/>
+    <mergeCell ref="B57:B63"/>
+    <mergeCell ref="B64:B72"/>
+    <mergeCell ref="B73:B77"/>
+    <mergeCell ref="A78:A90"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="A91:A97"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A98:A103"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="B104:B107"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>

</xml_diff>